<commit_message>
Amendments to xlsx and test summaries.
</commit_message>
<xml_diff>
--- a/tests/test_data/test.xlsx
+++ b/tests/test_data/test.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\t-hirose\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\t-hirose\dim\tests\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3F1CEC00-6E64-4414-9CA1-B705DDAD095B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29E503AA-F7D5-4A95-8C6E-9C875AA68B5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1770" windowWidth="21135" windowHeight="11895" xr2:uid="{156702D3-5BAF-40A3-BD98-435054AE20E8}"/>
+    <workbookView xWindow="1515" yWindow="2115" windowWidth="21135" windowHeight="11895" xr2:uid="{156702D3-5BAF-40A3-BD98-435054AE20E8}"/>
   </bookViews>
   <sheets>
     <sheet name="test" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>a</t>
     <phoneticPr fontId="1"/>
@@ -44,6 +44,18 @@
   </si>
   <si>
     <t>c</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>d</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>e</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>f</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -408,23 +420,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C9C8596-431F-4FA2-B961-F4754B820A5B}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A2" t="s">
         <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>